<commit_message>
updated programcreator, database, main.html
</commit_message>
<xml_diff>
--- a/dick.xlsx
+++ b/dick.xlsx
@@ -7,14 +7,14 @@
     <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Week 1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="40">
   <si>
     <t>WEEK 1</t>
   </si>
@@ -22,82 +22,118 @@
     <t>DAY 1</t>
   </si>
   <si>
-    <t>Close Grip Bench</t>
+    <t>Incline Press Machine</t>
+  </si>
+  <si>
+    <t>3x8</t>
+  </si>
+  <si>
+    <t>Rear Delt Flies</t>
+  </si>
+  <si>
+    <t>4x12</t>
+  </si>
+  <si>
+    <t>DB Press</t>
+  </si>
+  <si>
+    <t>3x6</t>
+  </si>
+  <si>
+    <t>Skullcrushers</t>
+  </si>
+  <si>
+    <t>Overhead Cable Extensions</t>
   </si>
   <si>
     <t>4x8</t>
   </si>
   <si>
-    <t>DB Front Raises</t>
+    <t>DAY 2</t>
+  </si>
+  <si>
+    <t>Seated Cable Rows</t>
+  </si>
+  <si>
+    <t>DB Rows</t>
+  </si>
+  <si>
+    <t>Straight Arm Lat Pulldowns</t>
+  </si>
+  <si>
+    <t>4x10</t>
+  </si>
+  <si>
+    <t>DB Curls</t>
+  </si>
+  <si>
+    <t>Waiter Curl</t>
+  </si>
+  <si>
+    <t>DAY 3</t>
+  </si>
+  <si>
+    <t>Quad Extensions</t>
+  </si>
+  <si>
+    <t>Hack Squat</t>
+  </si>
+  <si>
+    <t>Split Squats</t>
   </si>
   <si>
     <t>4x6</t>
   </si>
   <si>
-    <t>Incline Press Machine</t>
-  </si>
-  <si>
-    <t>Dips</t>
+    <t>Romanian Deadlifts</t>
+  </si>
+  <si>
+    <t>Hip Thrusts</t>
+  </si>
+  <si>
+    <t>DAY 4</t>
+  </si>
+  <si>
+    <t>Lateral Raises</t>
+  </si>
+  <si>
+    <t>Cable Flies</t>
   </si>
   <si>
     <t>3x12</t>
   </si>
   <si>
-    <t>Overhead Cable Extensions</t>
-  </si>
-  <si>
-    <t>3x6</t>
-  </si>
-  <si>
-    <t>DAY 2</t>
-  </si>
-  <si>
-    <t>4x10</t>
-  </si>
-  <si>
-    <t>Cable Flies</t>
+    <t>Tricep Kickbacks</t>
   </si>
   <si>
     <t>Rope Pushdowns</t>
   </si>
   <si>
-    <t>3x8</t>
-  </si>
-  <si>
-    <t>DAY 3</t>
-  </si>
-  <si>
-    <t>Incline DB Press</t>
-  </si>
-  <si>
-    <t>Lateral Raises</t>
-  </si>
-  <si>
-    <t>Skullcrushers</t>
+    <t>DAY 5</t>
+  </si>
+  <si>
+    <t>Barbell Rows</t>
+  </si>
+  <si>
+    <t>Lat Pulldowns</t>
   </si>
   <si>
     <t>3x10</t>
   </si>
   <si>
-    <t>DAY 4</t>
-  </si>
-  <si>
-    <t>Landmine Press</t>
-  </si>
-  <si>
-    <t>Tricep Kickbacks</t>
-  </si>
-  <si>
-    <t>DAY 5</t>
+    <t>Barbell Curls</t>
+  </si>
+  <si>
+    <t>Cable Curls</t>
   </si>
   <si>
     <t>DAY 6</t>
   </si>
   <si>
-    <t>Face Pulls</t>
-  </si>
-  <si>
-    <t>DB Press</t>
+    <t>Goblet Squat</t>
+  </si>
+  <si>
+    <t>Barbell Lunges</t>
   </si>
 </sst>
 </file>
@@ -573,17 +609,17 @@
       <c r="B9" s="2"/>
       <c r="C9" s="2"/>
       <c r="D9" s="3" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
     </row>
     <row r="10" spans="1:19">
       <c r="A10" s="3" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B10" s="2"/>
       <c r="C10" s="2"/>
       <c r="D10" s="3" t="s">
-        <v>8</v>
+        <v>3</v>
       </c>
     </row>
     <row r="11" spans="1:19">
@@ -604,17 +640,17 @@
     </row>
     <row r="16" spans="1:19">
       <c r="A16" s="3" t="s">
-        <v>2</v>
+        <v>12</v>
       </c>
       <c r="B16" s="2"/>
       <c r="C16" s="2"/>
       <c r="D16" s="3" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
     </row>
     <row r="17" spans="1:4">
       <c r="A17" s="3" t="s">
-        <v>4</v>
+        <v>13</v>
       </c>
       <c r="B17" s="2"/>
       <c r="C17" s="2"/>
@@ -624,236 +660,236 @@
     </row>
     <row r="18" spans="1:4">
       <c r="A18" s="3" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B18" s="2"/>
       <c r="C18" s="2"/>
       <c r="D18" s="3" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
     </row>
     <row r="19" spans="1:4">
       <c r="A19" s="3" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="B19" s="2"/>
       <c r="C19" s="2"/>
       <c r="D19" s="3" t="s">
-        <v>15</v>
+        <v>7</v>
       </c>
     </row>
     <row r="20" spans="1:4">
       <c r="A20" s="3" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="B20" s="2"/>
       <c r="C20" s="2"/>
       <c r="D20" s="3" t="s">
-        <v>3</v>
+        <v>15</v>
       </c>
     </row>
     <row r="23" spans="1:4">
       <c r="A23" s="2" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="B23" s="2"/>
     </row>
     <row r="25" spans="1:4">
       <c r="A25" s="3" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="B25" s="2"/>
       <c r="C25" s="2"/>
       <c r="D25" s="3" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
     </row>
     <row r="26" spans="1:4">
       <c r="A26" s="3" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="B26" s="2"/>
       <c r="C26" s="2"/>
       <c r="D26" s="3" t="s">
-        <v>15</v>
+        <v>7</v>
       </c>
     </row>
     <row r="27" spans="1:4">
       <c r="A27" s="3" t="s">
-        <v>6</v>
+        <v>21</v>
       </c>
       <c r="B27" s="2"/>
       <c r="C27" s="2"/>
       <c r="D27" s="3" t="s">
-        <v>15</v>
+        <v>22</v>
       </c>
     </row>
     <row r="28" spans="1:4">
       <c r="A28" s="3" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="B28" s="2"/>
       <c r="C28" s="2"/>
       <c r="D28" s="3" t="s">
-        <v>15</v>
+        <v>7</v>
       </c>
     </row>
     <row r="29" spans="1:4">
       <c r="A29" s="3" t="s">
-        <v>9</v>
+        <v>24</v>
       </c>
       <c r="B29" s="2"/>
       <c r="C29" s="2"/>
       <c r="D29" s="3" t="s">
-        <v>20</v>
+        <v>7</v>
       </c>
     </row>
     <row r="32" spans="1:4">
       <c r="A32" s="2" t="s">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="B32" s="2"/>
     </row>
     <row r="34" spans="1:4">
       <c r="A34" s="3" t="s">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="B34" s="2"/>
       <c r="C34" s="2"/>
       <c r="D34" s="3" t="s">
-        <v>3</v>
+        <v>22</v>
       </c>
     </row>
     <row r="35" spans="1:4">
       <c r="A35" s="3" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="B35" s="2"/>
       <c r="C35" s="2"/>
       <c r="D35" s="3" t="s">
-        <v>3</v>
+        <v>15</v>
       </c>
     </row>
     <row r="36" spans="1:4">
       <c r="A36" s="3" t="s">
-        <v>2</v>
+        <v>27</v>
       </c>
       <c r="B36" s="2"/>
       <c r="C36" s="2"/>
       <c r="D36" s="3" t="s">
-        <v>5</v>
+        <v>28</v>
       </c>
     </row>
     <row r="37" spans="1:4">
       <c r="A37" s="3" t="s">
-        <v>23</v>
+        <v>29</v>
       </c>
       <c r="B37" s="2"/>
       <c r="C37" s="2"/>
       <c r="D37" s="3" t="s">
-        <v>20</v>
+        <v>7</v>
       </c>
     </row>
     <row r="38" spans="1:4">
       <c r="A38" s="3" t="s">
-        <v>23</v>
+        <v>30</v>
       </c>
       <c r="B38" s="2"/>
       <c r="C38" s="2"/>
       <c r="D38" s="3" t="s">
-        <v>3</v>
+        <v>28</v>
       </c>
     </row>
     <row r="41" spans="1:4">
       <c r="A41" s="2" t="s">
-        <v>24</v>
+        <v>31</v>
       </c>
       <c r="B41" s="2"/>
     </row>
     <row r="43" spans="1:4">
       <c r="A43" s="3" t="s">
-        <v>2</v>
+        <v>12</v>
       </c>
       <c r="B43" s="2"/>
       <c r="C43" s="2"/>
       <c r="D43" s="3" t="s">
-        <v>20</v>
+        <v>7</v>
       </c>
     </row>
     <row r="44" spans="1:4">
       <c r="A44" s="3" t="s">
-        <v>22</v>
+        <v>32</v>
       </c>
       <c r="B44" s="2"/>
       <c r="C44" s="2"/>
       <c r="D44" s="3" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
     </row>
     <row r="45" spans="1:4">
       <c r="A45" s="3" t="s">
-        <v>13</v>
+        <v>33</v>
       </c>
       <c r="B45" s="2"/>
       <c r="C45" s="2"/>
       <c r="D45" s="3" t="s">
-        <v>20</v>
+        <v>34</v>
       </c>
     </row>
     <row r="46" spans="1:4">
       <c r="A46" s="3" t="s">
-        <v>14</v>
+        <v>35</v>
       </c>
       <c r="B46" s="2"/>
       <c r="C46" s="2"/>
       <c r="D46" s="3" t="s">
-        <v>3</v>
+        <v>22</v>
       </c>
     </row>
     <row r="47" spans="1:4">
       <c r="A47" s="3" t="s">
-        <v>9</v>
+        <v>36</v>
       </c>
       <c r="B47" s="2"/>
       <c r="C47" s="2"/>
       <c r="D47" s="3" t="s">
-        <v>3</v>
+        <v>10</v>
       </c>
     </row>
     <row r="50" spans="1:4">
       <c r="A50" s="2" t="s">
-        <v>25</v>
+        <v>37</v>
       </c>
       <c r="B50" s="2"/>
     </row>
     <row r="52" spans="1:4">
       <c r="A52" s="3" t="s">
-        <v>6</v>
+        <v>24</v>
       </c>
       <c r="B52" s="2"/>
       <c r="C52" s="2"/>
       <c r="D52" s="3" t="s">
-        <v>15</v>
+        <v>3</v>
       </c>
     </row>
     <row r="53" spans="1:4">
       <c r="A53" s="3" t="s">
-        <v>26</v>
+        <v>38</v>
       </c>
       <c r="B53" s="2"/>
       <c r="C53" s="2"/>
       <c r="D53" s="3" t="s">
-        <v>15</v>
+        <v>34</v>
       </c>
     </row>
     <row r="54" spans="1:4">
       <c r="A54" s="3" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="B54" s="2"/>
       <c r="C54" s="2"/>
       <c r="D54" s="3" t="s">
-        <v>5</v>
+        <v>28</v>
       </c>
     </row>
     <row r="55" spans="1:4">
@@ -863,17 +899,17 @@
       <c r="B55" s="2"/>
       <c r="C55" s="2"/>
       <c r="D55" s="3" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="56" spans="1:4">
       <c r="A56" s="3" t="s">
-        <v>14</v>
+        <v>39</v>
       </c>
       <c r="B56" s="2"/>
       <c r="C56" s="2"/>
       <c r="D56" s="3" t="s">
-        <v>3</v>
+        <v>34</v>
       </c>
     </row>
   </sheetData>

</xml_diff>